<commit_message>
Trends re-calculated based on precise data
</commit_message>
<xml_diff>
--- a/correlation-to-add.xlsx
+++ b/correlation-to-add.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rustam/Documents/Articles/InTheWorks/Ullmann/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429C93C4-BD4F-9542-AE9D-C64205245E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FA3A14-30E3-324B-8F43-8EB0571525FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{3443FCC9-A221-2F4C-8F82-5290AC19409C}"/>
   </bookViews>
@@ -88,8 +88,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC5C6"/>
       <color rgb="FFFFE4E4"/>
-      <color rgb="FFFFC5C6"/>
     </mruColors>
   </colors>
   <extLst>
@@ -156,7 +156,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C2152DE-F483-DA48-A4D3-891AD158A385}" type="CELLRANGE">
+                    <a:fld id="{5B4044E1-587C-5B42-8750-8E4FD76E4342}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -190,7 +190,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E20F4F9-234C-274F-9236-5B5B705B6B22}" type="CELLRANGE">
+                    <a:fld id="{5D68813D-833C-DF4B-8746-4C7F146D1F01}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -224,7 +224,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{221FF5C1-0882-B64E-82FA-9DCA0BF8BC21}" type="CELLRANGE">
+                    <a:fld id="{1D22CC25-B86A-6149-BAD6-C42A9DD0818C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -261,13 +261,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -318,13 +316,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.35</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -407,7 +405,8 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:backward val="0.4"/>
+            <c:forward val="0.1"/>
+            <c:backward val="0.5"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -418,13 +417,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.35</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,10 +490,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.0429999999999999</c:v>
+                  <c:v>1.026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32199999999999995</c:v>
+                  <c:v>0.35680000000000012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -547,7 +546,7 @@
                   <c:v>1.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57750000000000012</c:v>
+                  <c:v>0.63300000000000012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -600,7 +599,7 @@
                   <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97750000000000004</c:v>
+                  <c:v>1.0329999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,7 +615,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
@@ -653,7 +652,7 @@
                   <c:v>2.42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6475</c:v>
+                  <c:v>1.7029999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -681,6 +680,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -691,7 +691,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -705,13 +705,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Δ: phenyl-metal</a:t>
+                  <a:t>Δ: phenyl-metal binding enegy, eV</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> binding enegy, eV</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -728,7 +723,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -766,7 +761,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -797,11 +792,11 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -815,13 +810,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Energy of unassisted extraction</a:t>
+                  <a:t>Energy of unassisted extraction, eV</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>, eV</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -834,11 +824,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -876,7 +866,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -934,7 +924,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1800" b="0" i="0">
+        <a:defRPr sz="2000" b="0" i="0">
           <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
@@ -1061,7 +1051,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49B4CFD4-48F6-9847-AC6F-6832BE73A50B}" type="CELLRANGE">
+                    <a:fld id="{303C4439-05F2-A34E-84D0-682770F527FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1095,7 +1085,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F71A130-6D12-4342-A6D0-D2ED1AB62112}" type="CELLRANGE">
+                    <a:fld id="{3874007C-816B-D94A-96B8-C892502CB90B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1129,7 +1119,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97862748-4A80-7E43-A7F2-90DED08770AF}" type="CELLRANGE">
+                    <a:fld id="{769890F0-E86E-B44A-8EBC-E31160C1C6A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1219,13 +1209,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.35</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1307,13 +1297,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.35</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1380,10 +1370,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.0429999999999999</c:v>
+                  <c:v>1.026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32199999999999995</c:v>
+                  <c:v>0.35680000000000012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1436,7 +1426,7 @@
                   <c:v>1.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57750000000000012</c:v>
+                  <c:v>0.63300000000000012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1489,7 +1479,7 @@
                   <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97750000000000004</c:v>
+                  <c:v>1.0329999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,6 +1507,28 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-6076-CA45-AE10-0104043ADF14}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$18:$A$19</c:f>
@@ -1542,7 +1554,7 @@
                   <c:v>2.42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6475</c:v>
+                  <c:v>1.7029999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2885,13 +2897,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>756596</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>67554</xdr:rowOff>
+      <xdr:rowOff>67553</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>13511</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>178844</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3003,7 +3015,7 @@
       <cdr:y>0.64161</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.41677</cdr:x>
+      <cdr:x>0.43997</cdr:x>
       <cdr:y>0.7886</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -3019,8 +3031,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1028193" y="3070036"/>
-          <a:ext cx="2102562" cy="703314"/>
+          <a:off x="1033950" y="3292088"/>
+          <a:ext cx="2289730" cy="754203"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3032,7 +3044,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="2000" b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
@@ -3047,12 +3059,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.61502</cdr:x>
-      <cdr:y>0.45583</cdr:y>
+      <cdr:x>0.59709</cdr:x>
+      <cdr:y>0.50081</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.94295</cdr:x>
-      <cdr:y>0.58634</cdr:y>
+      <cdr:x>0.9522</cdr:x>
+      <cdr:y>0.63377</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3067,8 +3079,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4619959" y="2181098"/>
-          <a:ext cx="2463382" cy="624476"/>
+          <a:off x="4510547" y="2569624"/>
+          <a:ext cx="2682640" cy="682238"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3149,7 +3161,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="2000" b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
@@ -3164,12 +3176,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.20097</cdr:x>
-      <cdr:y>0.05526</cdr:y>
+      <cdr:x>0.16735</cdr:x>
+      <cdr:y>0.06819</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.63203</cdr:x>
-      <cdr:y>0.13019</cdr:y>
+      <cdr:x>0.63414</cdr:x>
+      <cdr:y>0.14367</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3184,8 +3196,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1509694" y="264414"/>
-          <a:ext cx="3238086" cy="358531"/>
+          <a:off x="1264177" y="349860"/>
+          <a:ext cx="3526298" cy="387286"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3263,7 +3275,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="2000" b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
@@ -3278,12 +3290,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.27721</cdr:x>
-      <cdr:y>0.35937</cdr:y>
+      <cdr:x>0.28086</cdr:x>
+      <cdr:y>0.35965</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.87002</cdr:x>
-      <cdr:y>0.43434</cdr:y>
+      <cdr:x>0.92281</cdr:x>
+      <cdr:y>0.43513</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3297,9 +3309,9 @@
         <cdr:cNvSpPr txBox="1"/>
       </cdr:nvSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="20700000">
-          <a:off x="2082402" y="1719535"/>
-          <a:ext cx="4453111" cy="358722"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="20640000">
+          <a:off x="2121653" y="1845367"/>
+          <a:ext cx="4849499" cy="387286"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3380,7 +3392,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1800" b="0" i="0">
+            <a:rPr lang="en-US" sz="2000" b="0" i="0">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
@@ -3400,12 +3412,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.08745</cdr:x>
-      <cdr:y>0.55228</cdr:y>
+      <cdr:x>0.08835</cdr:x>
+      <cdr:y>0.55916</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.8025</cdr:x>
-      <cdr:y>0.88424</cdr:y>
+      <cdr:x>0.83747</cdr:x>
+      <cdr:y>0.88554</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3420,8 +3432,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="601763" y="2948832"/>
-          <a:ext cx="4920617" cy="1772462"/>
+          <a:off x="605366" y="2991791"/>
+          <a:ext cx="5132915" cy="1746250"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rtTriangle">
           <a:avLst/>
@@ -3576,13 +3588,26 @@
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:schemeClr val="accent5">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-            <a:alpha val="90000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="67000">
+              <a:schemeClr val="bg1">
+                <a:alpha val="79000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="15000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+                <a:alpha val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect/>
+        </a:gradFill>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="1">
@@ -3671,12 +3696,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.09351</cdr:x>
-      <cdr:y>0.04598</cdr:y>
+      <cdr:x>0.08906</cdr:x>
+      <cdr:y>0.03252</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.77634</cdr:x>
-      <cdr:y>0.14161</cdr:y>
+      <cdr:x>0.80719</cdr:x>
+      <cdr:y>0.19952</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3691,21 +3716,35 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="642497" y="242900"/>
-          <a:ext cx="4691502" cy="505267"/>
+          <a:off x="610099" y="171802"/>
+          <a:ext cx="4919480" cy="882298"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr val="FFE4E4">
-            <a:alpha val="84000"/>
-          </a:srgbClr>
-        </a:solidFill>
+        <a:gradFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="bg1">
+                <a:alpha val="79000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="72000">
+              <a:srgbClr val="FFE2E3"/>
+            </a:gs>
+            <a:gs pos="15000">
+              <a:srgbClr val="FFC5C6">
+                <a:alpha val="74000"/>
+              </a:srgbClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+          <a:tileRect/>
+        </a:gradFill>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0" anchor="ctr" anchorCtr="1">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:lvl1pPr marL="0" indent="0">
@@ -3790,12 +3829,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.21225</cdr:x>
-      <cdr:y>0.35917</cdr:y>
+      <cdr:x>0.22206</cdr:x>
+      <cdr:y>0.36879</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.97207</cdr:x>
-      <cdr:y>0.46477</cdr:y>
+      <cdr:x>0.98188</cdr:x>
+      <cdr:y>0.47439</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3810,8 +3849,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="20640000">
-          <a:off x="1465494" y="1897587"/>
-          <a:ext cx="5246213" cy="557886"/>
+          <a:off x="1533227" y="1948367"/>
+          <a:ext cx="5246227" cy="557906"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4207,15 +4246,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB89E97D-DC6B-DB41-89B8-F06F9218ECE9}">
   <dimension ref="A2:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+    <sheetView tabSelected="1" topLeftCell="K4" zoomScale="125" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
       <c r="B2">
         <v>1.56</v>
@@ -4230,7 +4269,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0.85</v>
+        <v>0.89</v>
       </c>
       <c r="B3">
         <v>1.56</v>
@@ -4245,7 +4284,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.35</v>
+        <v>1.39</v>
       </c>
       <c r="B4">
         <v>1.76</v>
@@ -4263,7 +4302,7 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>1.0429999999999999</v>
+        <v>1.026</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4271,8 +4310,8 @@
         <v>1.4</v>
       </c>
       <c r="B8">
-        <f>$B$7-0.515*A8</f>
-        <v>0.32199999999999995</v>
+        <f>$B$7-0.478*A8</f>
+        <v>0.35680000000000012</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4280,8 +4319,8 @@
         <v>0.4</v>
       </c>
       <c r="B9">
-        <f>$B$7-0.515*A9</f>
-        <v>0.83699999999999997</v>
+        <f>$B$7-0.478*A9</f>
+        <v>0.83479999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4289,8 +4328,8 @@
         <v>0.85</v>
       </c>
       <c r="B10">
-        <f>$B$7-0.515*A10</f>
-        <v>0.60524999999999995</v>
+        <f>$B$7-0.478*A10</f>
+        <v>0.61970000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4306,8 +4345,8 @@
         <v>1.5</v>
       </c>
       <c r="B13">
-        <f>$B$12-0.515*A13</f>
-        <v>0.57750000000000012</v>
+        <f>$B$12-0.478*A13</f>
+        <v>0.63300000000000012</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4323,8 +4362,8 @@
         <v>1.5</v>
       </c>
       <c r="B16">
-        <f>$B$15-0.515*A16</f>
-        <v>0.97750000000000004</v>
+        <f>$B$15-0.478*A16</f>
+        <v>1.0329999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4340,8 +4379,8 @@
         <v>1.5</v>
       </c>
       <c r="B19">
-        <f>$B$18-0.515*A19</f>
-        <v>1.6475</v>
+        <f>$B$18-0.478*A19</f>
+        <v>1.7029999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>